<commit_message>
Register test case updated with real data.
</commit_message>
<xml_diff>
--- a/Tests/Test Cases/register.xlsx
+++ b/Tests/Test Cases/register.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/ALL/Master-BOUN/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3920" windowWidth="24000" windowHeight="13560"/>
+    <workbookView xWindow="-540" yWindow="960" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,6 @@
     <t>Registration is successfull popup shows up and user is directed to dashboard page.</t>
   </si>
   <si>
-    <t>1- Open register page.
-2- Enter all required information and bypass optional fields which are fields other than name, surname, email and password.</t>
-  </si>
-  <si>
     <t>#174, #175</t>
   </si>
   <si>
@@ -78,6 +74,14 @@
   </si>
   <si>
     <t>#176</t>
+  </si>
+  <si>
+    <t>1- Open register page.
+2- Enter name Hasancan
+3-Surname Akgunduz
+4-Email: hasancan@hotmail.com
+5-Password 123
+6-Click Save</t>
   </si>
 </sst>
 </file>
@@ -573,7 +577,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -618,7 +622,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -629,10 +633,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="1"/>
@@ -643,16 +647,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="1"/>

</xml_diff>